<commit_message>
updated results for 41473
</commit_message>
<xml_diff>
--- a/results/multilabel_powerset/41473ps/automl.xlsx
+++ b/results/multilabel_powerset/41473ps/automl.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
   <si>
     <t>f1_score_weighted</t>
   </si>
@@ -70,67 +70,76 @@
     <t>tpot</t>
   </si>
   <si>
-    <t>0.258 (0.238 ± 0.019)</t>
-  </si>
-  <si>
-    <t>0.209 (0.173 ± 0.018)</t>
-  </si>
-  <si>
-    <t>0.217 (0.171 ± 0.023)</t>
-  </si>
-  <si>
-    <t>0.230 (0.198 ± 0.018)</t>
-  </si>
-  <si>
-    <t>0.224 (0.157 ± 0.050)</t>
-  </si>
-  <si>
-    <t>0.180 (0.106 ± 0.044)</t>
-  </si>
-  <si>
-    <t>0.224 (0.191 ± 0.017)</t>
-  </si>
-  <si>
-    <t>0.213 (0.184 ± 0.017)</t>
-  </si>
-  <si>
-    <t>00:06:10 (00:27:23 ± 00:13:09)</t>
-  </si>
-  <si>
-    <t>00:01:00 (00:01:21 ± 00:00:19)</t>
-  </si>
-  <si>
-    <t>00:05:08 (00:05:16 ± 00:00:04)</t>
-  </si>
-  <si>
-    <t>00:04:57 (00:05:00 ± 00:00:03)</t>
-  </si>
-  <si>
-    <t>00:05:00 (00:05:07 ± 00:00:15)</t>
-  </si>
-  <si>
-    <t>00:05:16 (00:05:54 ± 00:00:26)</t>
-  </si>
-  <si>
-    <t>00:09:28 (00:09:48 ± 00:00:11)</t>
-  </si>
-  <si>
-    <t>00:05:18 (00:06:48 ± 00:01:27)</t>
-  </si>
-  <si>
-    <t>00:00:00 (00:00:02 ± 00:00:01)</t>
-  </si>
-  <si>
-    <t>00:00:00 (00:00:00 ± 00:00:00)</t>
-  </si>
-  <si>
-    <t>00:00:01 (00:00:02 ± 00:00:01)</t>
-  </si>
-  <si>
-    <t>00:00:01 (00:00:03 ± 00:00:02)</t>
+    <t>0.258 (0.238 Â± 0.019)</t>
+  </si>
+  <si>
+    <t>0.229 (0.191 Â± 0.021)</t>
+  </si>
+  <si>
+    <t>0.209 (0.173 Â± 0.018)</t>
+  </si>
+  <si>
+    <t>0.217 (0.171 Â± 0.023)</t>
+  </si>
+  <si>
+    <t>0.230 (0.198 Â± 0.018)</t>
+  </si>
+  <si>
+    <t>0.224 (0.157 Â± 0.050)</t>
+  </si>
+  <si>
+    <t>0.180 (0.106 Â± 0.044)</t>
+  </si>
+  <si>
+    <t>0.224 (0.191 Â± 0.017)</t>
+  </si>
+  <si>
+    <t>0.213 (0.184 Â± 0.017)</t>
+  </si>
+  <si>
+    <t>00:06:10 (00:27:23 Â± 00:13:09)</t>
+  </si>
+  <si>
+    <t>00:05:03 (00:06:33 Â± 00:01:07)</t>
+  </si>
+  <si>
+    <t>00:01:00 (00:01:21 Â± 00:00:19)</t>
+  </si>
+  <si>
+    <t>00:05:08 (00:05:16 Â± 00:00:04)</t>
+  </si>
+  <si>
+    <t>00:04:57 (00:05:00 Â± 00:00:03)</t>
+  </si>
+  <si>
+    <t>00:05:00 (00:05:07 Â± 00:00:15)</t>
+  </si>
+  <si>
+    <t>00:05:16 (00:05:54 Â± 00:00:26)</t>
+  </si>
+  <si>
+    <t>00:09:28 (00:09:48 Â± 00:00:11)</t>
+  </si>
+  <si>
+    <t>00:05:18 (00:06:48 Â± 00:01:27)</t>
+  </si>
+  <si>
+    <t>00:00:00 (00:00:02 Â± 00:00:01)</t>
+  </si>
+  <si>
+    <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
+  </si>
+  <si>
+    <t>00:00:01 (00:00:02 Â± 00:00:01)</t>
+  </si>
+  <si>
+    <t>00:00:01 (00:00:03 Â± 00:00:02)</t>
   </si>
   <si>
     <t>[]</t>
+  </si>
+  <si>
+    <t>59</t>
   </si>
   <si>
     <t>2</t>
@@ -537,13 +546,13 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F2">
         <v>13</v>
@@ -553,25 +562,40 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -579,19 +603,19 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -599,19 +623,19 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -624,19 +648,19 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -649,19 +673,19 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F10" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -674,19 +698,19 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F12" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -694,19 +718,19 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F13" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>